<commit_message>
Modelo de Ensamble MR
</commit_message>
<xml_diff>
--- a/Entregables/UdeBarcelona/models_Var_Lasso.xlsx
+++ b/Entregables/UdeBarcelona/models_Var_Lasso.xlsx
@@ -482,27 +482,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9859827176378499</v>
+        <v>0.985979005791894</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9236429557333753</v>
+        <v>0.9237427832909219</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06233976190447466</v>
+        <v>0.06223622250097216</v>
       </c>
       <c r="E2" t="n">
-        <v>3.883389399987074</v>
+        <v>3.883903536348642</v>
       </c>
       <c r="F2" t="n">
-        <v>9.063659553706772</v>
+        <v>9.057732799156215</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'solver': 'sag', 'alpha': 1.0}</t>
+          <t>{'solver': 'saga', 'alpha': 1.0}</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>4.13</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="3">
@@ -512,27 +512,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.986294233370364</v>
+        <v>0.986294271471534</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9246600335927929</v>
+        <v>0.9247897503465051</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06163419977757112</v>
+        <v>0.06150452112502891</v>
       </c>
       <c r="E3" t="n">
-        <v>3.839995330965513</v>
+        <v>3.839989993488935</v>
       </c>
       <c r="F3" t="n">
-        <v>9.003093097780862</v>
+        <v>8.99533921105319</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'selection': 'cyclic', 'alpha': 0.01}</t>
+          <t>{'selection': 'random', 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="4">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2.21</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="5">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>5.24</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="6">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5.14</v>
+        <v>6.55</v>
       </c>
     </row>
     <row r="7">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="8">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interpretación mejor modelo MR
</commit_message>
<xml_diff>
--- a/Entregables/UdeBarcelona/models_Var_Lasso.xlsx
+++ b/Entregables/UdeBarcelona/models_Var_Lasso.xlsx
@@ -482,19 +482,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.985979005791894</v>
+        <v>0.9859789073419475</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9237427832909219</v>
+        <v>0.9235314557650617</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06223622250097216</v>
+        <v>0.0624474515768858</v>
       </c>
       <c r="E2" t="n">
-        <v>3.883903536348642</v>
+        <v>3.883917171951741</v>
       </c>
       <c r="F2" t="n">
-        <v>9.057732799156215</v>
+        <v>9.070274720007825</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>3.96</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="3">
@@ -512,27 +512,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.986294271471534</v>
+        <v>0.986294233370364</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9247897503465051</v>
+        <v>0.9244396652579883</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06150452112502891</v>
+        <v>0.06185456811237577</v>
       </c>
       <c r="E3" t="n">
-        <v>3.839989993488935</v>
+        <v>3.839995330965513</v>
       </c>
       <c r="F3" t="n">
-        <v>8.99533921105319</v>
+        <v>9.016250443449955</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'selection': 'random', 'alpha': 0.01}</t>
+          <t>{'selection': 'cyclic', 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="4">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2.07</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="5">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>5.13</v>
+        <v>4.98</v>
       </c>
     </row>
     <row r="6">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>6.55</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="7">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2.15</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="8">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>